<commit_message>
add Types add Dbpedia.Searcher()
</commit_message>
<xml_diff>
--- a/Docs/Related_Work/state_of_art.xlsx
+++ b/Docs/Related_Work/state_of_art.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\apagado\tesis_Bicocca\Related_Work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ws\schema-annotation-workspace\schema-annotation\Docs\Related_Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C059D6-48E2-4A0B-A5B6-E4A5F550275A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF341E76-EAB7-4125-B30F-5E337DC825DC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="168" windowWidth="13824" windowHeight="7260" xr2:uid="{50CEE828-823E-4659-8ADD-46BC284A038B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{50CEE828-823E-4659-8ADD-46BC284A038B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="88">
   <si>
     <t>principal autor</t>
   </si>
@@ -302,6 +303,9 @@
   </si>
   <si>
     <t>Meta-Mappings for Sceham Mapping Reuse</t>
+  </si>
+  <si>
+    <t>LOV, LOD, Learning2Rank</t>
   </si>
 </sst>
 </file>
@@ -706,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9B52B68-1B2F-4FC4-A62B-523475A1D36A}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -907,6 +911,9 @@
       <c r="C8" s="7" t="s">
         <v>45</v>
       </c>
+      <c r="D8" s="6" t="s">
+        <v>87</v>
+      </c>
       <c r="E8" s="6" t="s">
         <v>45</v>
       </c>

</xml_diff>